<commit_message>
Version 1.0 fix bug.
</commit_message>
<xml_diff>
--- a/data/Hive_Map_Database2.xlsx
+++ b/data/Hive_Map_Database2.xlsx
@@ -15633,236 +15633,236 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="B3" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2">
-        <v>348.7444432128562</v>
+        <v>350.74550484845258</v>
       </c>
       <c r="E3" s="2">
-        <v>168.7444432128562</v>
+        <v>170.74550484845258</v>
       </c>
       <c r="F3" s="2">
-        <v>0.072017076417361381</v>
+        <v>0.019675075514620399</v>
       </c>
       <c r="G3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="2">
-        <v>10.000999999999999</v>
+        <v>7.0010000000000003</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B4" s="1">
         <v>8</v>
       </c>
       <c r="C4" s="1">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2">
+        <v>218.06988742113751</v>
+      </c>
+      <c r="E4" s="2">
+        <v>38.069887421137501</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.0083307846535043521</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>7.0010000000000003</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="1">
+        <v>1006</v>
+      </c>
+      <c r="B5" s="1">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1">
         <v>10</v>
       </c>
-      <c r="D4" s="2">
-        <v>350.74550484845258</v>
+      <c r="D5" s="2">
+        <v>358.69331543032581</v>
       </c>
-      <c r="E4" s="2">
-        <v>170.74550484845258</v>
+      <c r="E5" s="2">
+        <v>178.69331543032578</v>
       </c>
-      <c r="F4" s="2">
-        <v>0.019675075514620399</v>
+      <c r="F5" s="2">
+        <v>0.020347953788212133</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G5" s="3">
         <v>0</v>
       </c>
-      <c r="H4" s="2">
-        <v>7.0999999999999996</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1">
-        <v>1005</v>
-      </c>
-      <c r="B5" s="1">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2">
-        <v>218.06988742113751</v>
-      </c>
-      <c r="E5" s="2">
-        <v>38.069887421137501</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.0083307846535043521</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1</v>
-      </c>
       <c r="H5" s="2">
-        <v>7.0999999999999996</v>
+        <v>7.0010000000000003</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="B6" s="1">
         <v>7</v>
       </c>
       <c r="C6" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D6" s="2">
-        <v>358.69331543032581</v>
+        <v>168.69725918452605</v>
       </c>
       <c r="E6" s="2">
-        <v>178.69331543032578</v>
+        <v>348.69725918452605</v>
       </c>
       <c r="F6" s="2">
-        <v>0.020347953788212133</v>
+        <v>0.048203475614119973</v>
       </c>
       <c r="G6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="2">
-        <v>7.0999999999999996</v>
+        <v>7.0010000000000003</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="B7" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2">
-        <v>168.69725918452605</v>
+        <v>198.65774942341409</v>
       </c>
       <c r="E7" s="2">
-        <v>348.69725918452605</v>
+        <v>18.657749423414074</v>
       </c>
       <c r="F7" s="2">
-        <v>0.048203475614119973</v>
+        <v>0.030613089139273079</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
       </c>
       <c r="H7" s="2">
-        <v>7.0999999999999996</v>
+        <v>7.0010000000000003</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="B8" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="2">
-        <v>198.65774942341409</v>
+        <v>172.88762055557208</v>
       </c>
       <c r="E8" s="2">
-        <v>18.657749423414074</v>
+        <v>352.88762055557208</v>
       </c>
       <c r="F8" s="2">
-        <v>0.030613089139273079</v>
+        <v>0.053487017320475783</v>
       </c>
       <c r="G8" s="3">
         <v>1</v>
       </c>
       <c r="H8" s="2">
-        <v>7.0999999999999996</v>
+        <v>7.0010000000000003</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B9" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D9" s="2">
-        <v>172.88762055557208</v>
+        <v>111.93877624105005</v>
       </c>
       <c r="E9" s="2">
-        <v>352.88762055557208</v>
+        <v>291.93877624105005</v>
       </c>
       <c r="F9" s="2">
-        <v>0.053487017320475783</v>
+        <v>0.013610634551630163</v>
       </c>
       <c r="G9" s="3">
         <v>1</v>
       </c>
       <c r="H9" s="2">
-        <v>7.0999999999999996</v>
+        <v>7.0010000000000003</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="B10" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2">
-        <v>111.93877624105005</v>
+        <v>26.561640221446737</v>
       </c>
       <c r="E10" s="2">
-        <v>291.93877624105005</v>
+        <v>206.56164022144677</v>
       </c>
       <c r="F10" s="2">
-        <v>0.013610634551630163</v>
+        <v>0.025013067947655503</v>
       </c>
       <c r="G10" s="3">
         <v>1</v>
       </c>
       <c r="H10" s="2">
-        <v>7.0999999999999996</v>
+        <v>3.0009999999999999</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1">
-        <v>1011</v>
+        <v>1003</v>
       </c>
       <c r="B11" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D11" s="2">
-        <v>26.561640221446737</v>
+        <v>348.7444432128562</v>
       </c>
       <c r="E11" s="2">
-        <v>206.56164022144677</v>
+        <v>168.7444432128562</v>
       </c>
       <c r="F11" s="2">
-        <v>0.025013067947655503</v>
+        <v>0.072017076417361381</v>
       </c>
       <c r="G11" s="3">
         <v>1</v>
       </c>
       <c r="H11" s="2">
-        <v>3.0009999999999999</v>
+        <v>10.000999999999999</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">

</xml_diff>